<commit_message>
Add EMS_X in aggregation_rules.xlsx
</commit_message>
<xml_diff>
--- a/tests/Fred/bridges/aggregation_rules.xlsx
+++ b/tests/Fred/bridges/aggregation_rules.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reynesfgd\GitHub\ThreeME_V3\R_ThreeME\bridges\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reynesfgd\GitHub\ermeeth\tests\Fred\bridges\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78264090-0926-4252-8507-5FF1696DAF5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49E5F8CB-E9FA-4A59-A8F9-6C49FB933C3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8400" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-8400" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sectors" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="472">
   <si>
     <t>sum</t>
   </si>
@@ -1430,6 +1430,27 @@
   </si>
   <si>
     <t>C_n_VAL</t>
+  </si>
+  <si>
+    <t>EMS_X_CH4</t>
+  </si>
+  <si>
+    <t>EMS_X_CO2</t>
+  </si>
+  <si>
+    <t>EMS_X_HFC</t>
+  </si>
+  <si>
+    <t>EMS_X_N2O</t>
+  </si>
+  <si>
+    <t>EMS_X_PFC</t>
+  </si>
+  <si>
+    <t>EMS_X_SF6</t>
+  </si>
+  <si>
+    <t>EMS_X</t>
   </si>
 </sst>
 </file>
@@ -1786,8 +1807,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
-      <selection activeCell="H119" sqref="H119"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.25"/>
@@ -6366,10 +6390,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K268"/>
+  <dimension ref="A1:K275"/>
   <sheetViews>
-    <sheetView topLeftCell="A230" workbookViewId="0">
-      <selection activeCell="B251" sqref="B251"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B29" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.25"/>
@@ -7575,7 +7602,7 @@
     </row>
     <row r="53" spans="1:11">
       <c r="A53" s="4" t="s">
-        <v>297</v>
+        <v>471</v>
       </c>
       <c r="B53">
         <v>1</v>
@@ -7591,158 +7618,165 @@
         <v>#N/A</v>
       </c>
       <c r="G53" s="6"/>
-      <c r="H53" s="7"/>
-      <c r="I53" s="7"/>
-      <c r="J53" s="7"/>
-      <c r="K53" s="7"/>
+      <c r="H53" s="8"/>
+      <c r="I53" s="8"/>
+      <c r="J53" s="8"/>
+      <c r="K53" s="8"/>
     </row>
     <row r="54" spans="1:11">
       <c r="A54" s="4" t="s">
-        <v>298</v>
+        <v>465</v>
       </c>
       <c r="B54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C54">
         <v>0</v>
       </c>
       <c r="D54">
-        <v>1</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>274</v>
+        <v>0</v>
+      </c>
+      <c r="E54" s="2" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
       </c>
       <c r="G54" s="6"/>
-      <c r="H54" s="7"/>
-      <c r="I54" s="7"/>
-      <c r="J54" s="7"/>
-      <c r="K54" s="7"/>
+      <c r="H54" s="8"/>
+      <c r="I54" s="8"/>
+      <c r="J54" s="8"/>
+      <c r="K54" s="8"/>
     </row>
     <row r="55" spans="1:11">
       <c r="A55" s="4" t="s">
-        <v>69</v>
+        <v>466</v>
       </c>
       <c r="B55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C55">
         <v>0</v>
       </c>
       <c r="D55">
-        <v>1</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>43</v>
+        <v>0</v>
+      </c>
+      <c r="E55" s="2" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
       </c>
       <c r="G55" s="6"/>
-      <c r="H55" s="7"/>
-      <c r="I55" s="7"/>
-      <c r="J55" s="7"/>
-      <c r="K55" s="7"/>
+      <c r="H55" s="8"/>
+      <c r="I55" s="8"/>
+      <c r="J55" s="8"/>
+      <c r="K55" s="8"/>
     </row>
     <row r="56" spans="1:11">
       <c r="A56" s="4" t="s">
-        <v>299</v>
+        <v>467</v>
       </c>
       <c r="B56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C56">
         <v>0</v>
       </c>
       <c r="D56">
-        <v>1</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>306</v>
+        <v>0</v>
+      </c>
+      <c r="E56" s="2" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
       </c>
       <c r="G56" s="6"/>
-      <c r="H56" s="7"/>
-      <c r="I56" s="7"/>
-      <c r="J56" s="7"/>
-      <c r="K56" s="7"/>
+      <c r="H56" s="8"/>
+      <c r="I56" s="8"/>
+      <c r="J56" s="8"/>
+      <c r="K56" s="8"/>
     </row>
     <row r="57" spans="1:11">
       <c r="A57" s="4" t="s">
-        <v>74</v>
+        <v>468</v>
       </c>
       <c r="B57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C57">
         <v>0</v>
       </c>
       <c r="D57">
-        <v>1</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>125</v>
+        <v>0</v>
+      </c>
+      <c r="E57" s="2" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
       </c>
       <c r="G57" s="6"/>
-      <c r="H57" s="7"/>
-      <c r="I57" s="7"/>
-      <c r="J57" s="7"/>
-      <c r="K57" s="7"/>
+      <c r="H57" s="8"/>
+      <c r="I57" s="8"/>
+      <c r="J57" s="8"/>
+      <c r="K57" s="8"/>
     </row>
     <row r="58" spans="1:11">
       <c r="A58" s="4" t="s">
-        <v>300</v>
+        <v>469</v>
       </c>
       <c r="B58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C58">
         <v>0</v>
       </c>
       <c r="D58">
-        <v>1</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>322</v>
+        <v>0</v>
+      </c>
+      <c r="E58" s="2" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
       </c>
       <c r="G58" s="6"/>
-      <c r="H58" s="7"/>
-      <c r="I58" s="7"/>
-      <c r="J58" s="7"/>
-      <c r="K58" s="7"/>
+      <c r="H58" s="8"/>
+      <c r="I58" s="8"/>
+      <c r="J58" s="8"/>
+      <c r="K58" s="8"/>
     </row>
     <row r="59" spans="1:11">
       <c r="A59" s="4" t="s">
-        <v>301</v>
+        <v>470</v>
       </c>
       <c r="B59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C59">
         <v>0</v>
       </c>
       <c r="D59">
-        <v>1</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>454</v>
+        <v>0</v>
+      </c>
+      <c r="E59" s="2" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
       </c>
       <c r="G59" s="6"/>
-      <c r="H59" s="7"/>
-      <c r="I59" s="7"/>
-      <c r="J59" s="7"/>
-      <c r="K59" s="7"/>
+      <c r="H59" s="8"/>
+      <c r="I59" s="8"/>
+      <c r="J59" s="8"/>
+      <c r="K59" s="8"/>
     </row>
     <row r="60" spans="1:11">
       <c r="A60" s="4" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="B60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C60">
         <v>0</v>
       </c>
       <c r="D60">
-        <v>1</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>457</v>
+        <v>0</v>
+      </c>
+      <c r="E60" s="2" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
       </c>
       <c r="G60" s="6"/>
       <c r="H60" s="7"/>
@@ -7752,20 +7786,19 @@
     </row>
     <row r="61" spans="1:11">
       <c r="A61" s="4" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="B61">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C61">
         <v>0</v>
       </c>
       <c r="D61">
-        <v>0</v>
-      </c>
-      <c r="E61" s="2" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+        <v>1</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>274</v>
       </c>
       <c r="G61" s="6"/>
       <c r="H61" s="7"/>
@@ -7775,20 +7808,19 @@
     </row>
     <row r="62" spans="1:11">
       <c r="A62" s="4" t="s">
-        <v>304</v>
+        <v>69</v>
       </c>
       <c r="B62">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C62">
         <v>0</v>
       </c>
       <c r="D62">
-        <v>0</v>
-      </c>
-      <c r="E62" s="2" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+        <v>1</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="G62" s="6"/>
       <c r="H62" s="7"/>
@@ -7798,20 +7830,19 @@
     </row>
     <row r="63" spans="1:11">
       <c r="A63" s="4" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="B63">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C63">
         <v>0</v>
       </c>
       <c r="D63">
-        <v>0</v>
-      </c>
-      <c r="E63" s="2" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+        <v>1</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>306</v>
       </c>
       <c r="G63" s="6"/>
       <c r="H63" s="7"/>
@@ -7821,20 +7852,19 @@
     </row>
     <row r="64" spans="1:11">
       <c r="A64" s="4" t="s">
-        <v>306</v>
+        <v>74</v>
       </c>
       <c r="B64">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C64">
         <v>0</v>
       </c>
       <c r="D64">
-        <v>0</v>
-      </c>
-      <c r="E64" s="2" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+        <v>1</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>125</v>
       </c>
       <c r="G64" s="6"/>
       <c r="H64" s="7"/>
@@ -7844,20 +7874,19 @@
     </row>
     <row r="65" spans="1:11">
       <c r="A65" s="4" t="s">
-        <v>107</v>
+        <v>300</v>
       </c>
       <c r="B65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C65">
         <v>0</v>
       </c>
       <c r="D65">
-        <v>0</v>
-      </c>
-      <c r="E65" s="2" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+        <v>1</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>322</v>
       </c>
       <c r="G65" s="6"/>
       <c r="H65" s="7"/>
@@ -7867,20 +7896,19 @@
     </row>
     <row r="66" spans="1:11">
       <c r="A66" s="4" t="s">
-        <v>109</v>
+        <v>301</v>
       </c>
       <c r="B66">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C66">
         <v>0</v>
       </c>
       <c r="D66">
-        <v>0</v>
-      </c>
-      <c r="E66" s="2" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+        <v>1</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>454</v>
       </c>
       <c r="G66" s="6"/>
       <c r="H66" s="7"/>
@@ -7890,20 +7918,19 @@
     </row>
     <row r="67" spans="1:11">
       <c r="A67" s="4" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="B67">
         <v>0</v>
       </c>
       <c r="C67">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D67">
-        <v>0</v>
-      </c>
-      <c r="E67" s="2" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+        <v>1</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>457</v>
       </c>
       <c r="G67" s="6"/>
       <c r="H67" s="7"/>
@@ -7913,13 +7940,13 @@
     </row>
     <row r="68" spans="1:11">
       <c r="A68" s="4" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="B68">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D68">
         <v>0</v>
@@ -7936,13 +7963,13 @@
     </row>
     <row r="69" spans="1:11">
       <c r="A69" s="4" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="B69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C69">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D69">
         <v>0</v>
@@ -7959,13 +7986,13 @@
     </row>
     <row r="70" spans="1:11">
       <c r="A70" s="4" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="B70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C70">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D70">
         <v>0</v>
@@ -7982,13 +8009,13 @@
     </row>
     <row r="71" spans="1:11">
       <c r="A71" s="4" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="B71">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D71">
         <v>0</v>
@@ -8005,13 +8032,13 @@
     </row>
     <row r="72" spans="1:11">
       <c r="A72" s="4" t="s">
-        <v>312</v>
+        <v>107</v>
       </c>
       <c r="B72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C72">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D72">
         <v>0</v>
@@ -8028,13 +8055,13 @@
     </row>
     <row r="73" spans="1:11">
       <c r="A73" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C73">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D73">
         <v>0</v>
@@ -8051,7 +8078,7 @@
     </row>
     <row r="74" spans="1:11">
       <c r="A74" s="4" t="s">
-        <v>111</v>
+        <v>307</v>
       </c>
       <c r="B74">
         <v>0</v>
@@ -8074,7 +8101,7 @@
     </row>
     <row r="75" spans="1:11">
       <c r="A75" s="4" t="s">
-        <v>112</v>
+        <v>308</v>
       </c>
       <c r="B75">
         <v>0</v>
@@ -8097,13 +8124,13 @@
     </row>
     <row r="76" spans="1:11">
       <c r="A76" s="4" t="s">
-        <v>125</v>
+        <v>309</v>
       </c>
       <c r="B76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C76">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D76">
         <v>0</v>
@@ -8120,13 +8147,13 @@
     </row>
     <row r="77" spans="1:11">
       <c r="A77" s="4" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="B77">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C77">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D77">
         <v>0</v>
@@ -8143,13 +8170,13 @@
     </row>
     <row r="78" spans="1:11">
       <c r="A78" s="4" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="B78">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C78">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D78">
         <v>0</v>
@@ -8166,19 +8193,20 @@
     </row>
     <row r="79" spans="1:11">
       <c r="A79" s="4" t="s">
-        <v>126</v>
+        <v>312</v>
       </c>
       <c r="B79">
         <v>0</v>
       </c>
       <c r="C79">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D79">
-        <v>1</v>
-      </c>
-      <c r="E79" s="2" t="s">
-        <v>378</v>
+        <v>0</v>
+      </c>
+      <c r="E79" s="2" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
       </c>
       <c r="G79" s="6"/>
       <c r="H79" s="7"/>
@@ -8188,13 +8216,13 @@
     </row>
     <row r="80" spans="1:11">
       <c r="A80" s="4" t="s">
-        <v>315</v>
+        <v>110</v>
       </c>
       <c r="B80">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C80">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D80">
         <v>0</v>
@@ -8211,13 +8239,13 @@
     </row>
     <row r="81" spans="1:11">
       <c r="A81" s="4" t="s">
-        <v>316</v>
+        <v>111</v>
       </c>
       <c r="B81">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D81">
         <v>0</v>
@@ -8234,13 +8262,13 @@
     </row>
     <row r="82" spans="1:11">
       <c r="A82" s="4" t="s">
-        <v>317</v>
+        <v>112</v>
       </c>
       <c r="B82">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C82">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D82">
         <v>0</v>
@@ -8257,7 +8285,7 @@
     </row>
     <row r="83" spans="1:11">
       <c r="A83" s="4" t="s">
-        <v>318</v>
+        <v>125</v>
       </c>
       <c r="B83">
         <v>1</v>
@@ -8280,7 +8308,7 @@
     </row>
     <row r="84" spans="1:11">
       <c r="A84" s="4" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="B84">
         <v>1</v>
@@ -8303,7 +8331,7 @@
     </row>
     <row r="85" spans="1:11">
       <c r="A85" s="4" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="B85">
         <v>1</v>
@@ -8326,20 +8354,19 @@
     </row>
     <row r="86" spans="1:11">
       <c r="A86" s="4" t="s">
-        <v>321</v>
+        <v>126</v>
       </c>
       <c r="B86">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C86">
         <v>0</v>
       </c>
       <c r="D86">
-        <v>0</v>
-      </c>
-      <c r="E86" s="2" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+        <v>1</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>378</v>
       </c>
       <c r="G86" s="6"/>
       <c r="H86" s="7"/>
@@ -8349,7 +8376,7 @@
     </row>
     <row r="87" spans="1:11">
       <c r="A87" s="4" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="B87">
         <v>1</v>
@@ -8372,7 +8399,7 @@
     </row>
     <row r="88" spans="1:11">
       <c r="A88" s="4" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="B88">
         <v>1</v>
@@ -8395,7 +8422,7 @@
     </row>
     <row r="89" spans="1:11">
       <c r="A89" s="4" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="B89">
         <v>1</v>
@@ -8418,7 +8445,7 @@
     </row>
     <row r="90" spans="1:11">
       <c r="A90" s="4" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="B90">
         <v>1</v>
@@ -8441,7 +8468,7 @@
     </row>
     <row r="91" spans="1:11">
       <c r="A91" s="4" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="B91">
         <v>1</v>
@@ -8456,10 +8483,15 @@
         <f>NA()</f>
         <v>#N/A</v>
       </c>
+      <c r="G91" s="6"/>
+      <c r="H91" s="7"/>
+      <c r="I91" s="7"/>
+      <c r="J91" s="7"/>
+      <c r="K91" s="7"/>
     </row>
     <row r="92" spans="1:11">
       <c r="A92" s="4" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="B92">
         <v>1</v>
@@ -8474,10 +8506,15 @@
         <f>NA()</f>
         <v>#N/A</v>
       </c>
+      <c r="G92" s="6"/>
+      <c r="H92" s="7"/>
+      <c r="I92" s="7"/>
+      <c r="J92" s="7"/>
+      <c r="K92" s="7"/>
     </row>
     <row r="93" spans="1:11">
       <c r="A93" s="4" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="B93">
         <v>1</v>
@@ -8492,10 +8529,15 @@
         <f>NA()</f>
         <v>#N/A</v>
       </c>
+      <c r="G93" s="6"/>
+      <c r="H93" s="7"/>
+      <c r="I93" s="7"/>
+      <c r="J93" s="7"/>
+      <c r="K93" s="7"/>
     </row>
     <row r="94" spans="1:11">
       <c r="A94" s="4" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="B94">
         <v>1</v>
@@ -8510,10 +8552,15 @@
         <f>NA()</f>
         <v>#N/A</v>
       </c>
+      <c r="G94" s="6"/>
+      <c r="H94" s="7"/>
+      <c r="I94" s="7"/>
+      <c r="J94" s="7"/>
+      <c r="K94" s="7"/>
     </row>
     <row r="95" spans="1:11">
       <c r="A95" s="4" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="B95">
         <v>1</v>
@@ -8528,424 +8575,439 @@
         <f>NA()</f>
         <v>#N/A</v>
       </c>
+      <c r="G95" s="6"/>
+      <c r="H95" s="7"/>
+      <c r="I95" s="7"/>
+      <c r="J95" s="7"/>
+      <c r="K95" s="7"/>
     </row>
     <row r="96" spans="1:11">
       <c r="A96" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="B96">
+        <v>1</v>
+      </c>
+      <c r="C96">
+        <v>0</v>
+      </c>
+      <c r="D96">
+        <v>0</v>
+      </c>
+      <c r="E96" s="2" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G96" s="6"/>
+      <c r="H96" s="7"/>
+      <c r="I96" s="7"/>
+      <c r="J96" s="7"/>
+      <c r="K96" s="7"/>
+    </row>
+    <row r="97" spans="1:11">
+      <c r="A97" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="B97">
+        <v>1</v>
+      </c>
+      <c r="C97">
+        <v>0</v>
+      </c>
+      <c r="D97">
+        <v>0</v>
+      </c>
+      <c r="E97" s="2" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G97" s="6"/>
+      <c r="H97" s="7"/>
+      <c r="I97" s="7"/>
+      <c r="J97" s="7"/>
+      <c r="K97" s="7"/>
+    </row>
+    <row r="98" spans="1:11">
+      <c r="A98" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="B98">
+        <v>1</v>
+      </c>
+      <c r="C98">
+        <v>0</v>
+      </c>
+      <c r="D98">
+        <v>0</v>
+      </c>
+      <c r="E98" s="2" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11">
+      <c r="A99" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="B99">
+        <v>1</v>
+      </c>
+      <c r="C99">
+        <v>0</v>
+      </c>
+      <c r="D99">
+        <v>0</v>
+      </c>
+      <c r="E99" s="2" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11">
+      <c r="A100" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="B100">
+        <v>1</v>
+      </c>
+      <c r="C100">
+        <v>0</v>
+      </c>
+      <c r="D100">
+        <v>0</v>
+      </c>
+      <c r="E100" s="2" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11">
+      <c r="A101" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="B101">
+        <v>1</v>
+      </c>
+      <c r="C101">
+        <v>0</v>
+      </c>
+      <c r="D101">
+        <v>0</v>
+      </c>
+      <c r="E101" s="2" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11">
+      <c r="A102" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="B102">
+        <v>1</v>
+      </c>
+      <c r="C102">
+        <v>0</v>
+      </c>
+      <c r="D102">
+        <v>0</v>
+      </c>
+      <c r="E102" s="2" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11">
+      <c r="A103" s="4" t="s">
         <v>331</v>
       </c>
-      <c r="B96">
-        <v>1</v>
-      </c>
-      <c r="C96">
-        <v>0</v>
-      </c>
-      <c r="D96">
-        <v>0</v>
-      </c>
-      <c r="E96" s="2" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5">
-      <c r="A97" s="4" t="s">
+      <c r="B103">
+        <v>1</v>
+      </c>
+      <c r="C103">
+        <v>0</v>
+      </c>
+      <c r="D103">
+        <v>0</v>
+      </c>
+      <c r="E103" s="2" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11">
+      <c r="A104" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="B97">
-        <v>1</v>
-      </c>
-      <c r="C97">
-        <v>0</v>
-      </c>
-      <c r="D97">
-        <v>0</v>
-      </c>
-      <c r="E97" s="2" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5">
-      <c r="A98" s="4" t="s">
+      <c r="B104">
+        <v>1</v>
+      </c>
+      <c r="C104">
+        <v>0</v>
+      </c>
+      <c r="D104">
+        <v>0</v>
+      </c>
+      <c r="E104" s="2" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11">
+      <c r="A105" s="4" t="s">
         <v>333</v>
       </c>
-      <c r="B98">
-        <v>1</v>
-      </c>
-      <c r="C98">
-        <v>0</v>
-      </c>
-      <c r="D98">
-        <v>0</v>
-      </c>
-      <c r="E98" s="2" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5">
-      <c r="A99" s="4" t="s">
+      <c r="B105">
+        <v>1</v>
+      </c>
+      <c r="C105">
+        <v>0</v>
+      </c>
+      <c r="D105">
+        <v>0</v>
+      </c>
+      <c r="E105" s="2" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11">
+      <c r="A106" s="4" t="s">
         <v>334</v>
       </c>
-      <c r="B99">
-        <v>0</v>
-      </c>
-      <c r="C99">
-        <v>0</v>
-      </c>
-      <c r="D99">
-        <v>1</v>
-      </c>
-      <c r="E99" s="2" t="str">
-        <f>SUBSTITUTE(A99,"P","")</f>
+      <c r="B106">
+        <v>0</v>
+      </c>
+      <c r="C106">
+        <v>0</v>
+      </c>
+      <c r="D106">
+        <v>1</v>
+      </c>
+      <c r="E106" s="2" t="str">
+        <f>SUBSTITUTE(A106,"P","")</f>
         <v>CH</v>
       </c>
     </row>
-    <row r="100" spans="1:5">
-      <c r="A100" s="4" t="s">
+    <row r="107" spans="1:11">
+      <c r="A107" s="4" t="s">
         <v>335</v>
       </c>
-      <c r="B100">
-        <v>0</v>
-      </c>
-      <c r="C100">
-        <v>0</v>
-      </c>
-      <c r="D100">
-        <v>1</v>
-      </c>
-      <c r="E100" s="2" t="str">
-        <f t="shared" ref="E100:E111" si="0">SUBSTITUTE(A100,"P","")</f>
+      <c r="B107">
+        <v>0</v>
+      </c>
+      <c r="C107">
+        <v>0</v>
+      </c>
+      <c r="D107">
+        <v>1</v>
+      </c>
+      <c r="E107" s="2" t="str">
+        <f t="shared" ref="E107:E118" si="0">SUBSTITUTE(A107,"P","")</f>
         <v>CHD</v>
       </c>
     </row>
-    <row r="101" spans="1:5">
-      <c r="A101" s="4" t="s">
+    <row r="108" spans="1:11">
+      <c r="A108" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="B101">
-        <v>0</v>
-      </c>
-      <c r="C101">
-        <v>0</v>
-      </c>
-      <c r="D101">
-        <v>1</v>
-      </c>
-      <c r="E101" s="2" t="str">
+      <c r="B108">
+        <v>0</v>
+      </c>
+      <c r="C108">
+        <v>0</v>
+      </c>
+      <c r="D108">
+        <v>1</v>
+      </c>
+      <c r="E108" s="2" t="str">
         <f t="shared" si="0"/>
         <v>CHM</v>
       </c>
     </row>
-    <row r="102" spans="1:5">
-      <c r="A102" s="4" t="s">
+    <row r="109" spans="1:11">
+      <c r="A109" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="B102">
-        <v>0</v>
-      </c>
-      <c r="C102">
-        <v>0</v>
-      </c>
-      <c r="D102">
-        <v>1</v>
-      </c>
-      <c r="E102" s="2" t="str">
+      <c r="B109">
+        <v>0</v>
+      </c>
+      <c r="C109">
+        <v>0</v>
+      </c>
+      <c r="D109">
+        <v>1</v>
+      </c>
+      <c r="E109" s="2" t="str">
         <f t="shared" si="0"/>
         <v>CI</v>
       </c>
     </row>
-    <row r="103" spans="1:5">
-      <c r="A103" s="4" t="s">
+    <row r="110" spans="1:11">
+      <c r="A110" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="B103">
-        <v>0</v>
-      </c>
-      <c r="C103">
-        <v>0</v>
-      </c>
-      <c r="D103">
-        <v>1</v>
-      </c>
-      <c r="E103" s="2" t="str">
+      <c r="B110">
+        <v>0</v>
+      </c>
+      <c r="C110">
+        <v>0</v>
+      </c>
+      <c r="D110">
+        <v>1</v>
+      </c>
+      <c r="E110" s="2" t="str">
         <f t="shared" si="0"/>
         <v>CID</v>
       </c>
     </row>
-    <row r="104" spans="1:5">
-      <c r="A104" s="4" t="s">
+    <row r="111" spans="1:11">
+      <c r="A111" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="B104">
-        <v>0</v>
-      </c>
-      <c r="C104">
-        <v>0</v>
-      </c>
-      <c r="D104">
-        <v>1</v>
-      </c>
-      <c r="E104" s="2" t="str">
+      <c r="B111">
+        <v>0</v>
+      </c>
+      <c r="C111">
+        <v>0</v>
+      </c>
+      <c r="D111">
+        <v>1</v>
+      </c>
+      <c r="E111" s="2" t="str">
         <f t="shared" si="0"/>
         <v>CIM</v>
       </c>
     </row>
-    <row r="105" spans="1:5">
-      <c r="A105" s="4" t="s">
+    <row r="112" spans="1:11">
+      <c r="A112" s="4" t="s">
         <v>337</v>
       </c>
-      <c r="B105">
-        <v>0</v>
-      </c>
-      <c r="C105">
-        <v>0</v>
-      </c>
-      <c r="D105">
-        <v>1</v>
-      </c>
-      <c r="E105" s="2" t="str">
+      <c r="B112">
+        <v>0</v>
+      </c>
+      <c r="C112">
+        <v>0</v>
+      </c>
+      <c r="D112">
+        <v>1</v>
+      </c>
+      <c r="E112" s="2" t="str">
         <f t="shared" si="0"/>
         <v>DS</v>
       </c>
     </row>
-    <row r="106" spans="1:5">
-      <c r="A106" s="4" t="s">
+    <row r="113" spans="1:5">
+      <c r="A113" s="4" t="s">
         <v>338</v>
       </c>
-      <c r="B106">
-        <v>0</v>
-      </c>
-      <c r="C106">
-        <v>0</v>
-      </c>
-      <c r="D106">
-        <v>1</v>
-      </c>
-      <c r="E106" s="2" t="str">
+      <c r="B113">
+        <v>0</v>
+      </c>
+      <c r="C113">
+        <v>0</v>
+      </c>
+      <c r="D113">
+        <v>1</v>
+      </c>
+      <c r="E113" s="2" t="str">
         <f t="shared" si="0"/>
         <v>DSD</v>
       </c>
     </row>
-    <row r="107" spans="1:5">
-      <c r="A107" s="4" t="s">
+    <row r="114" spans="1:5">
+      <c r="A114" s="4" t="s">
         <v>339</v>
       </c>
-      <c r="B107">
-        <v>0</v>
-      </c>
-      <c r="C107">
-        <v>0</v>
-      </c>
-      <c r="D107">
-        <v>1</v>
-      </c>
-      <c r="E107" s="2" t="str">
+      <c r="B114">
+        <v>0</v>
+      </c>
+      <c r="C114">
+        <v>0</v>
+      </c>
+      <c r="D114">
+        <v>1</v>
+      </c>
+      <c r="E114" s="2" t="str">
         <f t="shared" si="0"/>
         <v>DSM</v>
       </c>
     </row>
-    <row r="108" spans="1:5">
-      <c r="A108" s="4" t="s">
+    <row r="115" spans="1:5">
+      <c r="A115" s="4" t="s">
         <v>340</v>
       </c>
-      <c r="B108">
-        <v>0</v>
-      </c>
-      <c r="C108">
-        <v>0</v>
-      </c>
-      <c r="D108">
-        <v>1</v>
-      </c>
-      <c r="E108" s="2" t="str">
+      <c r="B115">
+        <v>0</v>
+      </c>
+      <c r="C115">
+        <v>0</v>
+      </c>
+      <c r="D115">
+        <v>1</v>
+      </c>
+      <c r="E115" s="2" t="str">
         <f t="shared" si="0"/>
         <v>G</v>
       </c>
     </row>
-    <row r="109" spans="1:5">
-      <c r="A109" s="4" t="s">
+    <row r="116" spans="1:5">
+      <c r="A116" s="4" t="s">
         <v>341</v>
       </c>
-      <c r="B109">
-        <v>0</v>
-      </c>
-      <c r="C109">
-        <v>0</v>
-      </c>
-      <c r="D109">
-        <v>1</v>
-      </c>
-      <c r="E109" s="2" t="str">
+      <c r="B116">
+        <v>0</v>
+      </c>
+      <c r="C116">
+        <v>0</v>
+      </c>
+      <c r="D116">
+        <v>1</v>
+      </c>
+      <c r="E116" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GD</v>
       </c>
     </row>
-    <row r="110" spans="1:5">
-      <c r="A110" s="4" t="s">
+    <row r="117" spans="1:5">
+      <c r="A117" s="4" t="s">
         <v>342</v>
       </c>
-      <c r="B110">
-        <v>0</v>
-      </c>
-      <c r="C110">
-        <v>0</v>
-      </c>
-      <c r="D110">
-        <v>1</v>
-      </c>
-      <c r="E110" s="2" t="str">
+      <c r="B117">
+        <v>0</v>
+      </c>
+      <c r="C117">
+        <v>0</v>
+      </c>
+      <c r="D117">
+        <v>1</v>
+      </c>
+      <c r="E117" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GD</v>
       </c>
     </row>
-    <row r="111" spans="1:5">
-      <c r="A111" s="4" t="s">
+    <row r="118" spans="1:5">
+      <c r="A118" s="4" t="s">
         <v>343</v>
       </c>
-      <c r="B111">
-        <v>0</v>
-      </c>
-      <c r="C111">
-        <v>0</v>
-      </c>
-      <c r="D111">
-        <v>1</v>
-      </c>
-      <c r="E111" s="2" t="str">
+      <c r="B118">
+        <v>0</v>
+      </c>
+      <c r="C118">
+        <v>0</v>
+      </c>
+      <c r="D118">
+        <v>1</v>
+      </c>
+      <c r="E118" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GM</v>
       </c>
     </row>
-    <row r="112" spans="1:5">
-      <c r="A112" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="B112">
-        <v>0</v>
-      </c>
-      <c r="C112">
-        <v>1</v>
-      </c>
-      <c r="D112">
-        <v>0</v>
-      </c>
-      <c r="E112" s="2" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5">
-      <c r="A113" s="4" t="s">
-        <v>345</v>
-      </c>
-      <c r="B113">
-        <v>0</v>
-      </c>
-      <c r="C113">
-        <v>1</v>
-      </c>
-      <c r="D113">
-        <v>0</v>
-      </c>
-      <c r="E113" s="2" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5">
-      <c r="A114" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="B114">
-        <v>0</v>
-      </c>
-      <c r="C114">
-        <v>1</v>
-      </c>
-      <c r="D114">
-        <v>0</v>
-      </c>
-      <c r="E114" s="2" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5">
-      <c r="A115" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="B115">
-        <v>0</v>
-      </c>
-      <c r="C115">
-        <v>1</v>
-      </c>
-      <c r="D115">
-        <v>0</v>
-      </c>
-      <c r="E115" s="2" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5">
-      <c r="A116" s="4" t="s">
-        <v>346</v>
-      </c>
-      <c r="B116">
-        <v>0</v>
-      </c>
-      <c r="C116">
-        <v>1</v>
-      </c>
-      <c r="D116">
-        <v>0</v>
-      </c>
-      <c r="E116" s="2" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5">
-      <c r="A117" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="B117">
-        <v>0</v>
-      </c>
-      <c r="C117">
-        <v>1</v>
-      </c>
-      <c r="D117">
-        <v>0</v>
-      </c>
-      <c r="E117" s="2" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5">
-      <c r="A118" s="4" t="s">
-        <v>347</v>
-      </c>
-      <c r="B118">
-        <v>0</v>
-      </c>
-      <c r="C118">
-        <v>1</v>
-      </c>
-      <c r="D118">
-        <v>0</v>
-      </c>
-      <c r="E118" s="2" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-    </row>
     <row r="119" spans="1:5">
       <c r="A119" s="4" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="B119">
         <v>0</v>
@@ -8963,7 +9025,7 @@
     </row>
     <row r="120" spans="1:5">
       <c r="A120" s="4" t="s">
-        <v>145</v>
+        <v>345</v>
       </c>
       <c r="B120">
         <v>0</v>
@@ -8981,7 +9043,7 @@
     </row>
     <row r="121" spans="1:5">
       <c r="A121" s="4" t="s">
-        <v>349</v>
+        <v>139</v>
       </c>
       <c r="B121">
         <v>0</v>
@@ -8999,7 +9061,7 @@
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="4" t="s">
-        <v>257</v>
+        <v>140</v>
       </c>
       <c r="B122">
         <v>0</v>
@@ -9017,7 +9079,7 @@
     </row>
     <row r="123" spans="1:5">
       <c r="A123" s="4" t="s">
-        <v>138</v>
+        <v>346</v>
       </c>
       <c r="B123">
         <v>0</v>
@@ -9035,1091 +9097,1091 @@
     </row>
     <row r="124" spans="1:5">
       <c r="A124" s="4" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B124">
         <v>0</v>
       </c>
       <c r="C124">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D124">
-        <v>1</v>
-      </c>
-      <c r="E124" s="2" t="str">
-        <f>SUBSTITUTE(A124,"P","",1)</f>
-        <v>I</v>
+        <v>0</v>
+      </c>
+      <c r="E124" s="2" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="125" spans="1:5">
       <c r="A125" s="4" t="s">
-        <v>147</v>
+        <v>347</v>
       </c>
       <c r="B125">
         <v>0</v>
       </c>
       <c r="C125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D125">
-        <v>1</v>
-      </c>
-      <c r="E125" s="2" t="str">
-        <f t="shared" ref="E125:E154" si="1">SUBSTITUTE(A125,"P","",1)</f>
-        <v>ID</v>
+        <v>0</v>
+      </c>
+      <c r="E125" s="2" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="126" spans="1:5">
       <c r="A126" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="B126">
+        <v>0</v>
+      </c>
+      <c r="C126">
+        <v>1</v>
+      </c>
+      <c r="D126">
+        <v>0</v>
+      </c>
+      <c r="E126" s="2" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5">
+      <c r="A127" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B127">
+        <v>0</v>
+      </c>
+      <c r="C127">
+        <v>1</v>
+      </c>
+      <c r="D127">
+        <v>0</v>
+      </c>
+      <c r="E127" s="2" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5">
+      <c r="A128" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="B128">
+        <v>0</v>
+      </c>
+      <c r="C128">
+        <v>1</v>
+      </c>
+      <c r="D128">
+        <v>0</v>
+      </c>
+      <c r="E128" s="2" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5">
+      <c r="A129" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="B129">
+        <v>0</v>
+      </c>
+      <c r="C129">
+        <v>1</v>
+      </c>
+      <c r="D129">
+        <v>0</v>
+      </c>
+      <c r="E129" s="2" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5">
+      <c r="A130" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B130">
+        <v>0</v>
+      </c>
+      <c r="C130">
+        <v>1</v>
+      </c>
+      <c r="D130">
+        <v>0</v>
+      </c>
+      <c r="E130" s="2" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5">
+      <c r="A131" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B131">
+        <v>0</v>
+      </c>
+      <c r="C131">
+        <v>0</v>
+      </c>
+      <c r="D131">
+        <v>1</v>
+      </c>
+      <c r="E131" s="2" t="str">
+        <f>SUBSTITUTE(A131,"P","",1)</f>
+        <v>I</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5">
+      <c r="A132" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B132">
+        <v>0</v>
+      </c>
+      <c r="C132">
+        <v>0</v>
+      </c>
+      <c r="D132">
+        <v>1</v>
+      </c>
+      <c r="E132" s="2" t="str">
+        <f t="shared" ref="E132:E161" si="1">SUBSTITUTE(A132,"P","",1)</f>
+        <v>ID</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5">
+      <c r="A133" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="B126">
-        <v>0</v>
-      </c>
-      <c r="C126">
-        <v>0</v>
-      </c>
-      <c r="D126">
-        <v>1</v>
-      </c>
-      <c r="E126" s="2" t="str">
+      <c r="B133">
+        <v>0</v>
+      </c>
+      <c r="C133">
+        <v>0</v>
+      </c>
+      <c r="D133">
+        <v>1</v>
+      </c>
+      <c r="E133" s="2" t="str">
         <f t="shared" si="1"/>
         <v>IM</v>
       </c>
     </row>
-    <row r="127" spans="1:5">
-      <c r="A127" s="4" t="s">
+    <row r="134" spans="1:5">
+      <c r="A134" s="4" t="s">
         <v>350</v>
       </c>
-      <c r="B127">
-        <v>0</v>
-      </c>
-      <c r="C127">
-        <v>0</v>
-      </c>
-      <c r="D127">
-        <v>1</v>
-      </c>
-      <c r="E127" s="2" t="str">
+      <c r="B134">
+        <v>0</v>
+      </c>
+      <c r="C134">
+        <v>0</v>
+      </c>
+      <c r="D134">
+        <v>1</v>
+      </c>
+      <c r="E134" s="2" t="str">
         <f t="shared" si="1"/>
         <v>M</v>
       </c>
     </row>
-    <row r="128" spans="1:5">
-      <c r="A128" s="4" t="s">
+    <row r="135" spans="1:5">
+      <c r="A135" s="4" t="s">
         <v>351</v>
       </c>
-      <c r="B128">
-        <v>0</v>
-      </c>
-      <c r="C128">
-        <v>0</v>
-      </c>
-      <c r="D128">
-        <v>1</v>
-      </c>
-      <c r="E128" s="2" t="str">
+      <c r="B135">
+        <v>0</v>
+      </c>
+      <c r="C135">
+        <v>0</v>
+      </c>
+      <c r="D135">
+        <v>1</v>
+      </c>
+      <c r="E135" s="2" t="str">
         <f t="shared" si="1"/>
         <v>MBIS</v>
       </c>
     </row>
-    <row r="129" spans="1:5">
-      <c r="A129" s="4" t="s">
+    <row r="136" spans="1:5">
+      <c r="A136" s="4" t="s">
         <v>352</v>
       </c>
-      <c r="B129">
-        <v>0</v>
-      </c>
-      <c r="C129">
-        <v>0</v>
-      </c>
-      <c r="D129">
-        <v>1</v>
-      </c>
-      <c r="E129" s="2" t="str">
+      <c r="B136">
+        <v>0</v>
+      </c>
+      <c r="C136">
+        <v>0</v>
+      </c>
+      <c r="D136">
+        <v>1</v>
+      </c>
+      <c r="E136" s="2" t="str">
         <f t="shared" si="1"/>
         <v>MGPD</v>
       </c>
     </row>
-    <row r="130" spans="1:5">
-      <c r="A130" s="4" t="s">
+    <row r="137" spans="1:5">
+      <c r="A137" s="4" t="s">
         <v>353</v>
       </c>
-      <c r="B130">
-        <v>0</v>
-      </c>
-      <c r="C130">
-        <v>0</v>
-      </c>
-      <c r="D130">
-        <v>1</v>
-      </c>
-      <c r="E130" s="2" t="str">
+      <c r="B137">
+        <v>0</v>
+      </c>
+      <c r="C137">
+        <v>0</v>
+      </c>
+      <c r="D137">
+        <v>1</v>
+      </c>
+      <c r="E137" s="2" t="str">
         <f t="shared" si="1"/>
         <v>MGPM</v>
       </c>
     </row>
-    <row r="131" spans="1:5">
-      <c r="A131" s="4" t="s">
+    <row r="138" spans="1:5">
+      <c r="A138" s="4" t="s">
         <v>354</v>
       </c>
-      <c r="B131">
-        <v>0</v>
-      </c>
-      <c r="C131">
-        <v>0</v>
-      </c>
-      <c r="D131">
-        <v>1</v>
-      </c>
-      <c r="E131" s="2" t="str">
+      <c r="B138">
+        <v>0</v>
+      </c>
+      <c r="C138">
+        <v>0</v>
+      </c>
+      <c r="D138">
+        <v>1</v>
+      </c>
+      <c r="E138" s="2" t="str">
         <f t="shared" si="1"/>
         <v>MGS</v>
       </c>
     </row>
-    <row r="132" spans="1:5">
-      <c r="A132" s="4" t="s">
+    <row r="139" spans="1:5">
+      <c r="A139" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="B132">
-        <v>0</v>
-      </c>
-      <c r="C132">
-        <v>0</v>
-      </c>
-      <c r="D132">
-        <v>1</v>
-      </c>
-      <c r="E132" s="2" t="str">
+      <c r="B139">
+        <v>0</v>
+      </c>
+      <c r="C139">
+        <v>0</v>
+      </c>
+      <c r="D139">
+        <v>1</v>
+      </c>
+      <c r="E139" s="2" t="str">
         <f t="shared" si="1"/>
         <v>MGSBIS</v>
       </c>
     </row>
-    <row r="133" spans="1:5">
-      <c r="A133" s="4" t="s">
+    <row r="140" spans="1:5">
+      <c r="A140" s="4" t="s">
         <v>356</v>
       </c>
-      <c r="B133">
-        <v>0</v>
-      </c>
-      <c r="C133">
-        <v>0</v>
-      </c>
-      <c r="D133">
-        <v>1</v>
-      </c>
-      <c r="E133" s="2" t="str">
+      <c r="B140">
+        <v>0</v>
+      </c>
+      <c r="C140">
+        <v>0</v>
+      </c>
+      <c r="D140">
+        <v>1</v>
+      </c>
+      <c r="E140" s="2" t="str">
         <f t="shared" si="1"/>
         <v>MGSD</v>
       </c>
     </row>
-    <row r="134" spans="1:5">
-      <c r="A134" s="4" t="s">
+    <row r="141" spans="1:5">
+      <c r="A141" s="4" t="s">
         <v>357</v>
       </c>
-      <c r="B134">
-        <v>0</v>
-      </c>
-      <c r="C134">
-        <v>0</v>
-      </c>
-      <c r="D134">
-        <v>1</v>
-      </c>
-      <c r="E134" s="2" t="str">
+      <c r="B141">
+        <v>0</v>
+      </c>
+      <c r="C141">
+        <v>0</v>
+      </c>
+      <c r="D141">
+        <v>1</v>
+      </c>
+      <c r="E141" s="2" t="str">
         <f t="shared" si="1"/>
         <v>MGSM</v>
       </c>
     </row>
-    <row r="135" spans="1:5">
-      <c r="A135" s="4" t="s">
+    <row r="142" spans="1:5">
+      <c r="A142" s="4" t="s">
         <v>358</v>
       </c>
-      <c r="B135">
-        <v>0</v>
-      </c>
-      <c r="C135">
-        <v>0</v>
-      </c>
-      <c r="D135">
-        <v>1</v>
-      </c>
-      <c r="E135" s="2" t="str">
+      <c r="B142">
+        <v>0</v>
+      </c>
+      <c r="C142">
+        <v>0</v>
+      </c>
+      <c r="D142">
+        <v>1</v>
+      </c>
+      <c r="E142" s="2" t="str">
         <f t="shared" si="1"/>
         <v>MS</v>
       </c>
     </row>
-    <row r="136" spans="1:5">
-      <c r="A136" s="4" t="s">
+    <row r="143" spans="1:5">
+      <c r="A143" s="4" t="s">
         <v>359</v>
       </c>
-      <c r="B136">
-        <v>0</v>
-      </c>
-      <c r="C136">
-        <v>0</v>
-      </c>
-      <c r="D136">
-        <v>1</v>
-      </c>
-      <c r="E136" s="2" t="str">
+      <c r="B143">
+        <v>0</v>
+      </c>
+      <c r="C143">
+        <v>0</v>
+      </c>
+      <c r="D143">
+        <v>1</v>
+      </c>
+      <c r="E143" s="2" t="str">
         <f t="shared" si="1"/>
         <v>MSBVAT</v>
       </c>
     </row>
-    <row r="137" spans="1:5">
-      <c r="A137" s="4" t="s">
+    <row r="144" spans="1:5">
+      <c r="A144" s="4" t="s">
         <v>360</v>
       </c>
-      <c r="B137">
-        <v>0</v>
-      </c>
-      <c r="C137">
-        <v>0</v>
-      </c>
-      <c r="D137">
-        <v>1</v>
-      </c>
-      <c r="E137" s="2" t="str">
+      <c r="B144">
+        <v>0</v>
+      </c>
+      <c r="C144">
+        <v>0</v>
+      </c>
+      <c r="D144">
+        <v>1</v>
+      </c>
+      <c r="E144" s="2" t="str">
         <f t="shared" si="1"/>
         <v>NCH</v>
       </c>
     </row>
-    <row r="138" spans="1:5">
-      <c r="A138" s="4" t="s">
+    <row r="145" spans="1:5">
+      <c r="A145" s="4" t="s">
         <v>361</v>
       </c>
-      <c r="B138">
-        <v>0</v>
-      </c>
-      <c r="C138">
-        <v>0</v>
-      </c>
-      <c r="D138">
-        <v>1</v>
-      </c>
-      <c r="E138" s="2" t="str">
+      <c r="B145">
+        <v>0</v>
+      </c>
+      <c r="C145">
+        <v>0</v>
+      </c>
+      <c r="D145">
+        <v>1</v>
+      </c>
+      <c r="E145" s="2" t="str">
         <f t="shared" si="1"/>
         <v>OTHCTD</v>
       </c>
     </row>
-    <row r="139" spans="1:5">
-      <c r="A139" s="4" t="s">
+    <row r="146" spans="1:5">
+      <c r="A146" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="B139">
-        <v>0</v>
-      </c>
-      <c r="C139">
-        <v>0</v>
-      </c>
-      <c r="D139">
-        <v>1</v>
-      </c>
-      <c r="E139" s="2" t="str">
+      <c r="B146">
+        <v>0</v>
+      </c>
+      <c r="C146">
+        <v>0</v>
+      </c>
+      <c r="D146">
+        <v>1</v>
+      </c>
+      <c r="E146" s="2" t="str">
         <f t="shared" si="1"/>
         <v>OTHCTM</v>
       </c>
     </row>
-    <row r="140" spans="1:5">
-      <c r="A140" s="4" t="s">
+    <row r="147" spans="1:5">
+      <c r="A147" s="4" t="s">
         <v>363</v>
       </c>
-      <c r="B140">
-        <v>0</v>
-      </c>
-      <c r="C140">
-        <v>0</v>
-      </c>
-      <c r="D140">
-        <v>1</v>
-      </c>
-      <c r="E140" s="2" t="str">
+      <c r="B147">
+        <v>0</v>
+      </c>
+      <c r="C147">
+        <v>0</v>
+      </c>
+      <c r="D147">
+        <v>1</v>
+      </c>
+      <c r="E147" s="2" t="str">
         <f t="shared" si="1"/>
         <v>Q</v>
       </c>
     </row>
-    <row r="141" spans="1:5">
-      <c r="A141" s="4" t="s">
+    <row r="148" spans="1:5">
+      <c r="A148" s="4" t="s">
         <v>364</v>
       </c>
-      <c r="B141">
-        <v>0</v>
-      </c>
-      <c r="C141">
-        <v>0</v>
-      </c>
-      <c r="D141">
-        <v>1</v>
-      </c>
-      <c r="E141" s="2" t="str">
+      <c r="B148">
+        <v>0</v>
+      </c>
+      <c r="C148">
+        <v>0</v>
+      </c>
+      <c r="D148">
+        <v>1</v>
+      </c>
+      <c r="E148" s="2" t="str">
         <f t="shared" si="1"/>
         <v>QD</v>
       </c>
     </row>
-    <row r="142" spans="1:5">
-      <c r="A142" s="4" t="s">
+    <row r="149" spans="1:5">
+      <c r="A149" s="4" t="s">
         <v>365</v>
       </c>
-      <c r="B142">
-        <v>0</v>
-      </c>
-      <c r="C142">
-        <v>0</v>
-      </c>
-      <c r="D142">
-        <v>1</v>
-      </c>
-      <c r="E142" s="2" t="str">
+      <c r="B149">
+        <v>0</v>
+      </c>
+      <c r="C149">
+        <v>0</v>
+      </c>
+      <c r="D149">
+        <v>1</v>
+      </c>
+      <c r="E149" s="2" t="str">
         <f t="shared" si="1"/>
         <v>QM</v>
       </c>
     </row>
-    <row r="143" spans="1:5">
-      <c r="A143" s="4" t="s">
+    <row r="150" spans="1:5">
+      <c r="A150" s="4" t="s">
         <v>366</v>
       </c>
-      <c r="B143">
-        <v>0</v>
-      </c>
-      <c r="C143">
-        <v>0</v>
-      </c>
-      <c r="D143">
-        <v>1</v>
-      </c>
-      <c r="E143" s="2" t="str">
+      <c r="B150">
+        <v>0</v>
+      </c>
+      <c r="C150">
+        <v>0</v>
+      </c>
+      <c r="D150">
+        <v>1</v>
+      </c>
+      <c r="E150" s="2" t="str">
         <f t="shared" si="1"/>
         <v>SUBCD</v>
       </c>
     </row>
-    <row r="144" spans="1:5">
-      <c r="A144" s="4" t="s">
+    <row r="151" spans="1:5">
+      <c r="A151" s="4" t="s">
         <v>367</v>
       </c>
-      <c r="B144">
-        <v>0</v>
-      </c>
-      <c r="C144">
-        <v>0</v>
-      </c>
-      <c r="D144">
-        <v>1</v>
-      </c>
-      <c r="E144" s="2" t="str">
+      <c r="B151">
+        <v>0</v>
+      </c>
+      <c r="C151">
+        <v>0</v>
+      </c>
+      <c r="D151">
+        <v>1</v>
+      </c>
+      <c r="E151" s="2" t="str">
         <f t="shared" si="1"/>
         <v>SUBCM</v>
       </c>
     </row>
-    <row r="145" spans="1:5">
-      <c r="A145" s="4" t="s">
+    <row r="152" spans="1:5">
+      <c r="A152" s="4" t="s">
         <v>368</v>
       </c>
-      <c r="B145">
-        <v>0</v>
-      </c>
-      <c r="C145">
-        <v>0</v>
-      </c>
-      <c r="D145">
-        <v>1</v>
-      </c>
-      <c r="E145" s="2" t="str">
+      <c r="B152">
+        <v>0</v>
+      </c>
+      <c r="C152">
+        <v>0</v>
+      </c>
+      <c r="D152">
+        <v>1</v>
+      </c>
+      <c r="E152" s="2" t="str">
         <f t="shared" si="1"/>
         <v>VATD</v>
       </c>
     </row>
-    <row r="146" spans="1:5">
-      <c r="A146" s="4" t="s">
+    <row r="153" spans="1:5">
+      <c r="A153" s="4" t="s">
         <v>369</v>
       </c>
-      <c r="B146">
-        <v>0</v>
-      </c>
-      <c r="C146">
-        <v>0</v>
-      </c>
-      <c r="D146">
-        <v>1</v>
-      </c>
-      <c r="E146" s="2" t="str">
+      <c r="B153">
+        <v>0</v>
+      </c>
+      <c r="C153">
+        <v>0</v>
+      </c>
+      <c r="D153">
+        <v>1</v>
+      </c>
+      <c r="E153" s="2" t="str">
         <f t="shared" si="1"/>
         <v>VATM</v>
       </c>
     </row>
-    <row r="147" spans="1:5">
-      <c r="A147" s="4" t="s">
+    <row r="154" spans="1:5">
+      <c r="A154" s="4" t="s">
         <v>370</v>
       </c>
-      <c r="B147">
-        <v>0</v>
-      </c>
-      <c r="C147">
-        <v>0</v>
-      </c>
-      <c r="D147">
-        <v>1</v>
-      </c>
-      <c r="E147" s="2" t="str">
+      <c r="B154">
+        <v>0</v>
+      </c>
+      <c r="C154">
+        <v>0</v>
+      </c>
+      <c r="D154">
+        <v>1</v>
+      </c>
+      <c r="E154" s="2" t="str">
         <f t="shared" si="1"/>
         <v>WD</v>
       </c>
     </row>
-    <row r="148" spans="1:5">
-      <c r="A148" s="4" t="s">
+    <row r="155" spans="1:5">
+      <c r="A155" s="4" t="s">
         <v>371</v>
       </c>
-      <c r="B148">
-        <v>0</v>
-      </c>
-      <c r="C148">
-        <v>0</v>
-      </c>
-      <c r="D148">
-        <v>1</v>
-      </c>
-      <c r="E148" s="2" t="str">
+      <c r="B155">
+        <v>0</v>
+      </c>
+      <c r="C155">
+        <v>0</v>
+      </c>
+      <c r="D155">
+        <v>1</v>
+      </c>
+      <c r="E155" s="2" t="str">
         <f t="shared" si="1"/>
         <v>X</v>
       </c>
     </row>
-    <row r="149" spans="1:5">
-      <c r="A149" s="4" t="s">
+    <row r="156" spans="1:5">
+      <c r="A156" s="4" t="s">
         <v>372</v>
       </c>
-      <c r="B149">
-        <v>0</v>
-      </c>
-      <c r="C149">
-        <v>0</v>
-      </c>
-      <c r="D149">
-        <v>1</v>
-      </c>
-      <c r="E149" s="2" t="str">
+      <c r="B156">
+        <v>0</v>
+      </c>
+      <c r="C156">
+        <v>0</v>
+      </c>
+      <c r="D156">
+        <v>1</v>
+      </c>
+      <c r="E156" s="2" t="str">
         <f t="shared" si="1"/>
         <v>XD</v>
       </c>
     </row>
-    <row r="150" spans="1:5">
-      <c r="A150" s="4" t="s">
+    <row r="157" spans="1:5">
+      <c r="A157" s="4" t="s">
         <v>373</v>
       </c>
-      <c r="B150">
-        <v>0</v>
-      </c>
-      <c r="C150">
-        <v>0</v>
-      </c>
-      <c r="D150">
-        <v>1</v>
-      </c>
-      <c r="E150" s="2" t="str">
+      <c r="B157">
+        <v>0</v>
+      </c>
+      <c r="C157">
+        <v>0</v>
+      </c>
+      <c r="D157">
+        <v>1</v>
+      </c>
+      <c r="E157" s="2" t="str">
         <f t="shared" si="1"/>
         <v>XM</v>
       </c>
     </row>
-    <row r="151" spans="1:5">
-      <c r="A151" s="4" t="s">
+    <row r="158" spans="1:5">
+      <c r="A158" s="4" t="s">
         <v>374</v>
       </c>
-      <c r="B151">
-        <v>0</v>
-      </c>
-      <c r="C151">
-        <v>0</v>
-      </c>
-      <c r="D151">
-        <v>1</v>
-      </c>
-      <c r="E151" s="2" t="str">
+      <c r="B158">
+        <v>0</v>
+      </c>
+      <c r="C158">
+        <v>0</v>
+      </c>
+      <c r="D158">
+        <v>1</v>
+      </c>
+      <c r="E158" s="2" t="str">
         <f t="shared" si="1"/>
         <v>YQ</v>
       </c>
     </row>
-    <row r="152" spans="1:5">
-      <c r="A152" s="4" t="s">
+    <row r="159" spans="1:5">
+      <c r="A159" s="4" t="s">
         <v>375</v>
       </c>
-      <c r="B152">
-        <v>0</v>
-      </c>
-      <c r="C152">
-        <v>0</v>
-      </c>
-      <c r="D152">
-        <v>1</v>
-      </c>
-      <c r="E152" s="2" t="str">
+      <c r="B159">
+        <v>0</v>
+      </c>
+      <c r="C159">
+        <v>0</v>
+      </c>
+      <c r="D159">
+        <v>1</v>
+      </c>
+      <c r="E159" s="2" t="str">
         <f t="shared" si="1"/>
         <v>YQBIS</v>
       </c>
     </row>
-    <row r="153" spans="1:5">
-      <c r="A153" s="4" t="s">
+    <row r="160" spans="1:5">
+      <c r="A160" s="4" t="s">
         <v>376</v>
       </c>
-      <c r="B153">
-        <v>0</v>
-      </c>
-      <c r="C153">
-        <v>0</v>
-      </c>
-      <c r="D153">
-        <v>1</v>
-      </c>
-      <c r="E153" s="2" t="str">
+      <c r="B160">
+        <v>0</v>
+      </c>
+      <c r="C160">
+        <v>0</v>
+      </c>
+      <c r="D160">
+        <v>1</v>
+      </c>
+      <c r="E160" s="2" t="str">
         <f t="shared" si="1"/>
         <v>YQS</v>
       </c>
     </row>
-    <row r="154" spans="1:5">
-      <c r="A154" s="4" t="s">
+    <row r="161" spans="1:5">
+      <c r="A161" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="B154">
-        <v>0</v>
-      </c>
-      <c r="C154">
-        <v>0</v>
-      </c>
-      <c r="D154">
-        <v>1</v>
-      </c>
-      <c r="E154" s="2" t="str">
+      <c r="B161">
+        <v>0</v>
+      </c>
+      <c r="C161">
+        <v>0</v>
+      </c>
+      <c r="D161">
+        <v>1</v>
+      </c>
+      <c r="E161" s="2" t="str">
         <f t="shared" si="1"/>
         <v>YQSBVAT</v>
       </c>
     </row>
-    <row r="155" spans="1:5">
-      <c r="A155" s="4" t="s">
+    <row r="162" spans="1:5">
+      <c r="A162" s="4" t="s">
         <v>378</v>
       </c>
-      <c r="B155">
-        <v>1</v>
-      </c>
-      <c r="C155">
-        <v>0</v>
-      </c>
-      <c r="D155">
-        <v>0</v>
-      </c>
-      <c r="E155" s="2" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5">
-      <c r="A156" s="4" t="s">
+      <c r="B162">
+        <v>1</v>
+      </c>
+      <c r="C162">
+        <v>0</v>
+      </c>
+      <c r="D162">
+        <v>0</v>
+      </c>
+      <c r="E162" s="2" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5">
+      <c r="A163" s="4" t="s">
         <v>379</v>
       </c>
-      <c r="B156">
-        <v>1</v>
-      </c>
-      <c r="C156">
-        <v>0</v>
-      </c>
-      <c r="D156">
-        <v>0</v>
-      </c>
-      <c r="E156" s="2" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="157" spans="1:5">
-      <c r="A157" s="4" t="s">
+      <c r="B163">
+        <v>1</v>
+      </c>
+      <c r="C163">
+        <v>0</v>
+      </c>
+      <c r="D163">
+        <v>0</v>
+      </c>
+      <c r="E163" s="2" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5">
+      <c r="A164" s="4" t="s">
         <v>380</v>
       </c>
-      <c r="B157">
-        <v>1</v>
-      </c>
-      <c r="C157">
-        <v>0</v>
-      </c>
-      <c r="D157">
-        <v>0</v>
-      </c>
-      <c r="E157" s="2" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5">
-      <c r="A158" s="4" t="s">
+      <c r="B164">
+        <v>1</v>
+      </c>
+      <c r="C164">
+        <v>0</v>
+      </c>
+      <c r="D164">
+        <v>0</v>
+      </c>
+      <c r="E164" s="2" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5">
+      <c r="A165" s="4" t="s">
         <v>381</v>
       </c>
-      <c r="B158">
-        <v>0</v>
-      </c>
-      <c r="C158">
-        <v>0</v>
-      </c>
-      <c r="D158">
-        <v>1</v>
-      </c>
-      <c r="E158" s="2" t="str">
-        <f>SUBSTITUTE(A158,"R2","EMS")</f>
+      <c r="B165">
+        <v>0</v>
+      </c>
+      <c r="C165">
+        <v>0</v>
+      </c>
+      <c r="D165">
+        <v>1</v>
+      </c>
+      <c r="E165" s="2" t="str">
+        <f>SUBSTITUTE(A165,"R2","EMS")</f>
         <v>EMS_CH_CH4</v>
       </c>
     </row>
-    <row r="159" spans="1:5">
-      <c r="A159" s="4" t="s">
+    <row r="166" spans="1:5">
+      <c r="A166" s="4" t="s">
         <v>382</v>
       </c>
-      <c r="B159">
-        <v>0</v>
-      </c>
-      <c r="C159">
-        <v>0</v>
-      </c>
-      <c r="D159">
-        <v>1</v>
-      </c>
-      <c r="E159" s="2" t="str">
-        <f t="shared" ref="E159:E166" si="2">SUBSTITUTE(A159,"R2","EMS")</f>
+      <c r="B166">
+        <v>0</v>
+      </c>
+      <c r="C166">
+        <v>0</v>
+      </c>
+      <c r="D166">
+        <v>1</v>
+      </c>
+      <c r="E166" s="2" t="str">
+        <f t="shared" ref="E166:E173" si="2">SUBSTITUTE(A166,"R2","EMS")</f>
         <v>EMS_CH_CO2</v>
       </c>
     </row>
-    <row r="160" spans="1:5">
-      <c r="A160" s="4" t="s">
+    <row r="167" spans="1:5">
+      <c r="A167" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="B160">
-        <v>0</v>
-      </c>
-      <c r="C160">
-        <v>0</v>
-      </c>
-      <c r="D160">
-        <v>1</v>
-      </c>
-      <c r="E160" s="2" t="str">
+      <c r="B167">
+        <v>0</v>
+      </c>
+      <c r="C167">
+        <v>0</v>
+      </c>
+      <c r="D167">
+        <v>1</v>
+      </c>
+      <c r="E167" s="2" t="str">
         <f t="shared" si="2"/>
         <v>EMS_CH_HFC</v>
       </c>
     </row>
-    <row r="161" spans="1:5">
-      <c r="A161" s="4" t="s">
+    <row r="168" spans="1:5">
+      <c r="A168" s="4" t="s">
         <v>384</v>
       </c>
-      <c r="B161">
-        <v>0</v>
-      </c>
-      <c r="C161">
-        <v>0</v>
-      </c>
-      <c r="D161">
-        <v>1</v>
-      </c>
-      <c r="E161" s="2" t="str">
+      <c r="B168">
+        <v>0</v>
+      </c>
+      <c r="C168">
+        <v>0</v>
+      </c>
+      <c r="D168">
+        <v>1</v>
+      </c>
+      <c r="E168" s="2" t="str">
         <f t="shared" si="2"/>
         <v>EMS_CH_N2O</v>
       </c>
     </row>
-    <row r="162" spans="1:5">
-      <c r="A162" s="4" t="s">
+    <row r="169" spans="1:5">
+      <c r="A169" s="4" t="s">
         <v>385</v>
       </c>
-      <c r="B162">
-        <v>0</v>
-      </c>
-      <c r="C162">
-        <v>0</v>
-      </c>
-      <c r="D162">
-        <v>1</v>
-      </c>
-      <c r="E162" s="2" t="str">
+      <c r="B169">
+        <v>0</v>
+      </c>
+      <c r="C169">
+        <v>0</v>
+      </c>
+      <c r="D169">
+        <v>1</v>
+      </c>
+      <c r="E169" s="2" t="str">
         <f t="shared" si="2"/>
         <v>EMS_CH_PFC</v>
       </c>
     </row>
-    <row r="163" spans="1:5">
-      <c r="A163" s="4" t="s">
+    <row r="170" spans="1:5">
+      <c r="A170" s="4" t="s">
         <v>386</v>
       </c>
-      <c r="B163">
-        <v>0</v>
-      </c>
-      <c r="C163">
-        <v>0</v>
-      </c>
-      <c r="D163">
-        <v>1</v>
-      </c>
-      <c r="E163" s="2" t="str">
+      <c r="B170">
+        <v>0</v>
+      </c>
+      <c r="C170">
+        <v>0</v>
+      </c>
+      <c r="D170">
+        <v>1</v>
+      </c>
+      <c r="E170" s="2" t="str">
         <f t="shared" si="2"/>
         <v>EMS_CH_SF6</v>
       </c>
     </row>
-    <row r="164" spans="1:5">
-      <c r="A164" s="4" t="s">
+    <row r="171" spans="1:5">
+      <c r="A171" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="B164">
-        <v>0</v>
-      </c>
-      <c r="C164">
-        <v>0</v>
-      </c>
-      <c r="D164">
-        <v>1</v>
-      </c>
-      <c r="E164" s="2" t="str">
+      <c r="B171">
+        <v>0</v>
+      </c>
+      <c r="C171">
+        <v>0</v>
+      </c>
+      <c r="D171">
+        <v>1</v>
+      </c>
+      <c r="E171" s="2" t="str">
         <f t="shared" si="2"/>
         <v>EMS_CI_CH4</v>
       </c>
     </row>
-    <row r="165" spans="1:5">
-      <c r="A165" s="4" t="s">
+    <row r="172" spans="1:5">
+      <c r="A172" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="B165">
-        <v>0</v>
-      </c>
-      <c r="C165">
-        <v>0</v>
-      </c>
-      <c r="D165">
-        <v>1</v>
-      </c>
-      <c r="E165" s="2" t="str">
+      <c r="B172">
+        <v>0</v>
+      </c>
+      <c r="C172">
+        <v>0</v>
+      </c>
+      <c r="D172">
+        <v>1</v>
+      </c>
+      <c r="E172" s="2" t="str">
         <f t="shared" si="2"/>
         <v>EMS_CI_CO2</v>
       </c>
     </row>
-    <row r="166" spans="1:5">
-      <c r="A166" s="4" t="s">
+    <row r="173" spans="1:5">
+      <c r="A173" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="B166">
-        <v>0</v>
-      </c>
-      <c r="C166">
-        <v>0</v>
-      </c>
-      <c r="D166">
-        <v>1</v>
-      </c>
-      <c r="E166" s="2" t="str">
+      <c r="B173">
+        <v>0</v>
+      </c>
+      <c r="C173">
+        <v>0</v>
+      </c>
+      <c r="D173">
+        <v>1</v>
+      </c>
+      <c r="E173" s="2" t="str">
         <f t="shared" si="2"/>
         <v>EMS_CI_N2O</v>
       </c>
     </row>
-    <row r="167" spans="1:5">
-      <c r="A167" s="4" t="s">
+    <row r="174" spans="1:5">
+      <c r="A174" s="4" t="s">
         <v>387</v>
       </c>
-      <c r="B167">
-        <v>0</v>
-      </c>
-      <c r="C167">
-        <v>0</v>
-      </c>
-      <c r="D167">
-        <v>1</v>
-      </c>
-      <c r="E167" s="2" t="s">
+      <c r="B174">
+        <v>0</v>
+      </c>
+      <c r="C174">
+        <v>0</v>
+      </c>
+      <c r="D174">
+        <v>1</v>
+      </c>
+      <c r="E174" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="168" spans="1:5">
-      <c r="A168" s="4" t="s">
+    <row r="175" spans="1:5">
+      <c r="A175" s="4" t="s">
         <v>388</v>
       </c>
-      <c r="B168">
-        <v>0</v>
-      </c>
-      <c r="C168">
-        <v>0</v>
-      </c>
-      <c r="D168">
-        <v>1</v>
-      </c>
-      <c r="E168" s="2" t="s">
+      <c r="B175">
+        <v>0</v>
+      </c>
+      <c r="C175">
+        <v>0</v>
+      </c>
+      <c r="D175">
+        <v>1</v>
+      </c>
+      <c r="E175" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="169" spans="1:5">
-      <c r="A169" s="4" t="s">
+    <row r="176" spans="1:5">
+      <c r="A176" s="4" t="s">
         <v>389</v>
       </c>
-      <c r="B169">
-        <v>0</v>
-      </c>
-      <c r="C169">
-        <v>0</v>
-      </c>
-      <c r="D169">
-        <v>1</v>
-      </c>
-      <c r="E169" s="2" t="str">
-        <f>SUBSTITUTE(A169,"R","")</f>
+      <c r="B176">
+        <v>0</v>
+      </c>
+      <c r="C176">
+        <v>0</v>
+      </c>
+      <c r="D176">
+        <v>1</v>
+      </c>
+      <c r="E176" s="2" t="str">
+        <f>SUBSTITUTE(A176,"R","")</f>
         <v>NTAXCD</v>
       </c>
     </row>
-    <row r="170" spans="1:5">
-      <c r="A170" s="4" t="s">
+    <row r="177" spans="1:5">
+      <c r="A177" s="4" t="s">
         <v>390</v>
       </c>
-      <c r="B170">
-        <v>0</v>
-      </c>
-      <c r="C170">
-        <v>0</v>
-      </c>
-      <c r="D170">
-        <v>1</v>
-      </c>
-      <c r="E170" s="2" t="str">
-        <f t="shared" ref="E170:E176" si="3">SUBSTITUTE(A170,"R","")</f>
+      <c r="B177">
+        <v>0</v>
+      </c>
+      <c r="C177">
+        <v>0</v>
+      </c>
+      <c r="D177">
+        <v>1</v>
+      </c>
+      <c r="E177" s="2" t="str">
+        <f t="shared" ref="E177:E183" si="3">SUBSTITUTE(A177,"R","")</f>
         <v>NTAXCM</v>
       </c>
     </row>
-    <row r="171" spans="1:5">
-      <c r="A171" s="4" t="s">
+    <row r="178" spans="1:5">
+      <c r="A178" s="4" t="s">
         <v>391</v>
       </c>
-      <c r="B171">
-        <v>0</v>
-      </c>
-      <c r="C171">
-        <v>0</v>
-      </c>
-      <c r="D171">
-        <v>1</v>
-      </c>
-      <c r="E171" s="2" t="str">
+      <c r="B178">
+        <v>0</v>
+      </c>
+      <c r="C178">
+        <v>0</v>
+      </c>
+      <c r="D178">
+        <v>1</v>
+      </c>
+      <c r="E178" s="2" t="str">
         <f t="shared" si="3"/>
         <v>OTHCTD</v>
       </c>
     </row>
-    <row r="172" spans="1:5">
-      <c r="A172" s="4" t="s">
+    <row r="179" spans="1:5">
+      <c r="A179" s="4" t="s">
         <v>392</v>
       </c>
-      <c r="B172">
-        <v>0</v>
-      </c>
-      <c r="C172">
-        <v>0</v>
-      </c>
-      <c r="D172">
-        <v>1</v>
-      </c>
-      <c r="E172" s="2" t="str">
+      <c r="B179">
+        <v>0</v>
+      </c>
+      <c r="C179">
+        <v>0</v>
+      </c>
+      <c r="D179">
+        <v>1</v>
+      </c>
+      <c r="E179" s="2" t="str">
         <f t="shared" si="3"/>
         <v>OTHCTM</v>
       </c>
     </row>
-    <row r="173" spans="1:5">
-      <c r="A173" s="4" t="s">
+    <row r="180" spans="1:5">
+      <c r="A180" s="4" t="s">
         <v>393</v>
       </c>
-      <c r="B173">
-        <v>0</v>
-      </c>
-      <c r="C173">
-        <v>0</v>
-      </c>
-      <c r="D173">
-        <v>1</v>
-      </c>
-      <c r="E173" s="2" t="str">
+      <c r="B180">
+        <v>0</v>
+      </c>
+      <c r="C180">
+        <v>0</v>
+      </c>
+      <c r="D180">
+        <v>1</v>
+      </c>
+      <c r="E180" s="2" t="str">
         <f t="shared" si="3"/>
         <v>SUBCD</v>
       </c>
     </row>
-    <row r="174" spans="1:5">
-      <c r="A174" s="4" t="s">
+    <row r="181" spans="1:5">
+      <c r="A181" s="4" t="s">
         <v>394</v>
       </c>
-      <c r="B174">
-        <v>0</v>
-      </c>
-      <c r="C174">
-        <v>0</v>
-      </c>
-      <c r="D174">
-        <v>1</v>
-      </c>
-      <c r="E174" s="2" t="str">
+      <c r="B181">
+        <v>0</v>
+      </c>
+      <c r="C181">
+        <v>0</v>
+      </c>
+      <c r="D181">
+        <v>1</v>
+      </c>
+      <c r="E181" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VATD</v>
       </c>
     </row>
-    <row r="175" spans="1:5">
-      <c r="A175" s="4" t="s">
+    <row r="182" spans="1:5">
+      <c r="A182" s="4" t="s">
         <v>395</v>
       </c>
-      <c r="B175">
-        <v>0</v>
-      </c>
-      <c r="C175">
-        <v>0</v>
-      </c>
-      <c r="D175">
-        <v>1</v>
-      </c>
-      <c r="E175" s="2" t="str">
+      <c r="B182">
+        <v>0</v>
+      </c>
+      <c r="C182">
+        <v>0</v>
+      </c>
+      <c r="D182">
+        <v>1</v>
+      </c>
+      <c r="E182" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VATM</v>
       </c>
     </row>
-    <row r="176" spans="1:5">
-      <c r="A176" s="4" t="s">
+    <row r="183" spans="1:5">
+      <c r="A183" s="4" t="s">
         <v>396</v>
       </c>
-      <c r="B176">
-        <v>0</v>
-      </c>
-      <c r="C176">
-        <v>0</v>
-      </c>
-      <c r="D176">
-        <v>1</v>
-      </c>
-      <c r="E176" s="2" t="str">
+      <c r="B183">
+        <v>0</v>
+      </c>
+      <c r="C183">
+        <v>0</v>
+      </c>
+      <c r="D183">
+        <v>1</v>
+      </c>
+      <c r="E183" s="2" t="str">
         <f t="shared" si="3"/>
         <v>Y_TOE</v>
       </c>
     </row>
-    <row r="177" spans="1:5">
-      <c r="A177" s="4" t="s">
-        <v>397</v>
-      </c>
-      <c r="B177">
-        <v>1</v>
-      </c>
-      <c r="C177">
-        <v>0</v>
-      </c>
-      <c r="D177">
-        <v>0</v>
-      </c>
-      <c r="E177" s="2" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="178" spans="1:5">
-      <c r="A178" s="4" t="s">
-        <v>398</v>
-      </c>
-      <c r="B178">
-        <v>1</v>
-      </c>
-      <c r="C178">
-        <v>0</v>
-      </c>
-      <c r="D178">
-        <v>0</v>
-      </c>
-      <c r="E178" s="2" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="179" spans="1:5">
-      <c r="A179" s="4" t="s">
-        <v>399</v>
-      </c>
-      <c r="B179">
-        <v>0</v>
-      </c>
-      <c r="C179">
-        <v>1</v>
-      </c>
-      <c r="D179">
-        <v>0</v>
-      </c>
-      <c r="E179" s="2" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="180" spans="1:5">
-      <c r="A180" s="4" t="s">
-        <v>400</v>
-      </c>
-      <c r="B180">
-        <v>0</v>
-      </c>
-      <c r="C180">
-        <v>1</v>
-      </c>
-      <c r="D180">
-        <v>0</v>
-      </c>
-      <c r="E180" s="2" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="181" spans="1:5">
-      <c r="A181" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="B181">
-        <v>0</v>
-      </c>
-      <c r="C181">
-        <v>1</v>
-      </c>
-      <c r="D181">
-        <v>0</v>
-      </c>
-      <c r="E181" s="2" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="182" spans="1:5">
-      <c r="A182" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="B182">
-        <v>0</v>
-      </c>
-      <c r="C182">
-        <v>1</v>
-      </c>
-      <c r="D182">
-        <v>0</v>
-      </c>
-      <c r="E182" s="2" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="183" spans="1:5">
-      <c r="A183" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="B183">
-        <v>0</v>
-      </c>
-      <c r="C183">
-        <v>1</v>
-      </c>
-      <c r="D183">
-        <v>0</v>
-      </c>
-      <c r="E183" s="2" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-    </row>
     <row r="184" spans="1:5">
       <c r="A184" s="4" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="B184">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C184">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D184">
         <v>0</v>
@@ -10131,13 +10193,13 @@
     </row>
     <row r="185" spans="1:5">
       <c r="A185" s="4" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="B185">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C185">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D185">
         <v>0</v>
@@ -10149,7 +10211,7 @@
     </row>
     <row r="186" spans="1:5">
       <c r="A186" s="4" t="s">
-        <v>204</v>
+        <v>399</v>
       </c>
       <c r="B186">
         <v>0</v>
@@ -10167,7 +10229,7 @@
     </row>
     <row r="187" spans="1:5">
       <c r="A187" s="4" t="s">
-        <v>205</v>
+        <v>400</v>
       </c>
       <c r="B187">
         <v>0</v>
@@ -10185,7 +10247,7 @@
     </row>
     <row r="188" spans="1:5">
       <c r="A188" s="4" t="s">
-        <v>403</v>
+        <v>194</v>
       </c>
       <c r="B188">
         <v>0</v>
@@ -10203,7 +10265,7 @@
     </row>
     <row r="189" spans="1:5">
       <c r="A189" s="4" t="s">
-        <v>404</v>
+        <v>192</v>
       </c>
       <c r="B189">
         <v>0</v>
@@ -10221,7 +10283,7 @@
     </row>
     <row r="190" spans="1:5">
       <c r="A190" s="4" t="s">
-        <v>405</v>
+        <v>193</v>
       </c>
       <c r="B190">
         <v>0</v>
@@ -10239,7 +10301,7 @@
     </row>
     <row r="191" spans="1:5">
       <c r="A191" s="4" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="B191">
         <v>0</v>
@@ -10257,7 +10319,7 @@
     </row>
     <row r="192" spans="1:5">
       <c r="A192" s="4" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="B192">
         <v>0</v>
@@ -10275,7 +10337,7 @@
     </row>
     <row r="193" spans="1:5">
       <c r="A193" s="4" t="s">
-        <v>408</v>
+        <v>204</v>
       </c>
       <c r="B193">
         <v>0</v>
@@ -10293,7 +10355,7 @@
     </row>
     <row r="194" spans="1:5">
       <c r="A194" s="4" t="s">
-        <v>409</v>
+        <v>205</v>
       </c>
       <c r="B194">
         <v>0</v>
@@ -10311,7 +10373,7 @@
     </row>
     <row r="195" spans="1:5">
       <c r="A195" s="4" t="s">
-        <v>410</v>
+        <v>403</v>
       </c>
       <c r="B195">
         <v>0</v>
@@ -10329,7 +10391,7 @@
     </row>
     <row r="196" spans="1:5">
       <c r="A196" s="4" t="s">
-        <v>411</v>
+        <v>404</v>
       </c>
       <c r="B196">
         <v>0</v>
@@ -10347,7 +10409,7 @@
     </row>
     <row r="197" spans="1:5">
       <c r="A197" s="4" t="s">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="B197">
         <v>0</v>
@@ -10365,7 +10427,7 @@
     </row>
     <row r="198" spans="1:5">
       <c r="A198" s="4" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
       <c r="B198">
         <v>0</v>
@@ -10383,7 +10445,7 @@
     </row>
     <row r="199" spans="1:5">
       <c r="A199" s="4" t="s">
-        <v>414</v>
+        <v>407</v>
       </c>
       <c r="B199">
         <v>0</v>
@@ -10401,7 +10463,7 @@
     </row>
     <row r="200" spans="1:5">
       <c r="A200" s="4" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
       <c r="B200">
         <v>0</v>
@@ -10419,7 +10481,7 @@
     </row>
     <row r="201" spans="1:5">
       <c r="A201" s="4" t="s">
-        <v>228</v>
+        <v>409</v>
       </c>
       <c r="B201">
         <v>0</v>
@@ -10437,7 +10499,7 @@
     </row>
     <row r="202" spans="1:5">
       <c r="A202" s="4" t="s">
-        <v>229</v>
+        <v>410</v>
       </c>
       <c r="B202">
         <v>0</v>
@@ -10455,7 +10517,7 @@
     </row>
     <row r="203" spans="1:5">
       <c r="A203" s="4" t="s">
-        <v>230</v>
+        <v>411</v>
       </c>
       <c r="B203">
         <v>0</v>
@@ -10473,7 +10535,7 @@
     </row>
     <row r="204" spans="1:5">
       <c r="A204" s="4" t="s">
-        <v>231</v>
+        <v>412</v>
       </c>
       <c r="B204">
         <v>0</v>
@@ -10491,7 +10553,7 @@
     </row>
     <row r="205" spans="1:5">
       <c r="A205" s="4" t="s">
-        <v>232</v>
+        <v>413</v>
       </c>
       <c r="B205">
         <v>0</v>
@@ -10509,7 +10571,7 @@
     </row>
     <row r="206" spans="1:5">
       <c r="A206" s="4" t="s">
-        <v>233</v>
+        <v>414</v>
       </c>
       <c r="B206">
         <v>0</v>
@@ -10527,7 +10589,7 @@
     </row>
     <row r="207" spans="1:5">
       <c r="A207" s="4" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B207">
         <v>0</v>
@@ -10545,7 +10607,7 @@
     </row>
     <row r="208" spans="1:5">
       <c r="A208" s="4" t="s">
-        <v>417</v>
+        <v>228</v>
       </c>
       <c r="B208">
         <v>0</v>
@@ -10563,7 +10625,7 @@
     </row>
     <row r="209" spans="1:5">
       <c r="A209" s="4" t="s">
-        <v>418</v>
+        <v>229</v>
       </c>
       <c r="B209">
         <v>0</v>
@@ -10581,7 +10643,7 @@
     </row>
     <row r="210" spans="1:5">
       <c r="A210" s="4" t="s">
-        <v>419</v>
+        <v>230</v>
       </c>
       <c r="B210">
         <v>0</v>
@@ -10599,7 +10661,7 @@
     </row>
     <row r="211" spans="1:5">
       <c r="A211" s="4" t="s">
-        <v>420</v>
+        <v>231</v>
       </c>
       <c r="B211">
         <v>0</v>
@@ -10617,7 +10679,7 @@
     </row>
     <row r="212" spans="1:5">
       <c r="A212" s="4" t="s">
-        <v>421</v>
+        <v>232</v>
       </c>
       <c r="B212">
         <v>0</v>
@@ -10635,7 +10697,7 @@
     </row>
     <row r="213" spans="1:5">
       <c r="A213" s="4" t="s">
-        <v>422</v>
+        <v>233</v>
       </c>
       <c r="B213">
         <v>0</v>
@@ -10653,7 +10715,7 @@
     </row>
     <row r="214" spans="1:5">
       <c r="A214" s="4" t="s">
-        <v>423</v>
+        <v>416</v>
       </c>
       <c r="B214">
         <v>0</v>
@@ -10671,7 +10733,7 @@
     </row>
     <row r="215" spans="1:5">
       <c r="A215" s="4" t="s">
-        <v>424</v>
+        <v>417</v>
       </c>
       <c r="B215">
         <v>0</v>
@@ -10689,7 +10751,7 @@
     </row>
     <row r="216" spans="1:5">
       <c r="A216" s="4" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
       <c r="B216">
         <v>0</v>
@@ -10707,7 +10769,7 @@
     </row>
     <row r="217" spans="1:5">
       <c r="A217" s="4" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
       <c r="B217">
         <v>0</v>
@@ -10725,7 +10787,7 @@
     </row>
     <row r="218" spans="1:5">
       <c r="A218" s="4" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="B218">
         <v>0</v>
@@ -10743,7 +10805,7 @@
     </row>
     <row r="219" spans="1:5">
       <c r="A219" s="4" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="B219">
         <v>0</v>
@@ -10761,7 +10823,7 @@
     </row>
     <row r="220" spans="1:5">
       <c r="A220" s="4" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
       <c r="B220">
         <v>0</v>
@@ -10779,7 +10841,7 @@
     </row>
     <row r="221" spans="1:5">
       <c r="A221" s="4" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
       <c r="B221">
         <v>0</v>
@@ -10797,7 +10859,7 @@
     </row>
     <row r="222" spans="1:5">
       <c r="A222" s="4" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="B222">
         <v>0</v>
@@ -10815,7 +10877,7 @@
     </row>
     <row r="223" spans="1:5">
       <c r="A223" s="4" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
       <c r="B223">
         <v>0</v>
@@ -10833,7 +10895,7 @@
     </row>
     <row r="224" spans="1:5">
       <c r="A224" s="4" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
       <c r="B224">
         <v>0</v>
@@ -10851,7 +10913,7 @@
     </row>
     <row r="225" spans="1:5">
       <c r="A225" s="4" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="B225">
         <v>0</v>
@@ -10869,7 +10931,7 @@
     </row>
     <row r="226" spans="1:5">
       <c r="A226" s="4" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="B226">
         <v>0</v>
@@ -10887,7 +10949,7 @@
     </row>
     <row r="227" spans="1:5">
       <c r="A227" s="4" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
       <c r="B227">
         <v>0</v>
@@ -10905,7 +10967,7 @@
     </row>
     <row r="228" spans="1:5">
       <c r="A228" s="4" t="s">
-        <v>206</v>
+        <v>430</v>
       </c>
       <c r="B228">
         <v>0</v>
@@ -10923,7 +10985,7 @@
     </row>
     <row r="229" spans="1:5">
       <c r="A229" s="4" t="s">
-        <v>207</v>
+        <v>431</v>
       </c>
       <c r="B229">
         <v>0</v>
@@ -10941,7 +11003,7 @@
     </row>
     <row r="230" spans="1:5">
       <c r="A230" s="4" t="s">
-        <v>208</v>
+        <v>432</v>
       </c>
       <c r="B230">
         <v>0</v>
@@ -10959,7 +11021,7 @@
     </row>
     <row r="231" spans="1:5">
       <c r="A231" s="4" t="s">
-        <v>209</v>
+        <v>433</v>
       </c>
       <c r="B231">
         <v>0</v>
@@ -10977,7 +11039,7 @@
     </row>
     <row r="232" spans="1:5">
       <c r="A232" s="4" t="s">
-        <v>210</v>
+        <v>434</v>
       </c>
       <c r="B232">
         <v>0</v>
@@ -10995,7 +11057,7 @@
     </row>
     <row r="233" spans="1:5">
       <c r="A233" s="4" t="s">
-        <v>211</v>
+        <v>435</v>
       </c>
       <c r="B233">
         <v>0</v>
@@ -11013,7 +11075,7 @@
     </row>
     <row r="234" spans="1:5">
       <c r="A234" s="4" t="s">
-        <v>212</v>
+        <v>436</v>
       </c>
       <c r="B234">
         <v>0</v>
@@ -11031,7 +11093,7 @@
     </row>
     <row r="235" spans="1:5">
       <c r="A235" s="4" t="s">
-        <v>437</v>
+        <v>206</v>
       </c>
       <c r="B235">
         <v>0</v>
@@ -11049,7 +11111,7 @@
     </row>
     <row r="236" spans="1:5">
       <c r="A236" s="4" t="s">
-        <v>438</v>
+        <v>207</v>
       </c>
       <c r="B236">
         <v>0</v>
@@ -11067,7 +11129,7 @@
     </row>
     <row r="237" spans="1:5">
       <c r="A237" s="4" t="s">
-        <v>439</v>
+        <v>208</v>
       </c>
       <c r="B237">
         <v>0</v>
@@ -11085,7 +11147,7 @@
     </row>
     <row r="238" spans="1:5">
       <c r="A238" s="4" t="s">
-        <v>440</v>
+        <v>209</v>
       </c>
       <c r="B238">
         <v>0</v>
@@ -11103,7 +11165,7 @@
     </row>
     <row r="239" spans="1:5">
       <c r="A239" s="4" t="s">
-        <v>441</v>
+        <v>210</v>
       </c>
       <c r="B239">
         <v>0</v>
@@ -11121,7 +11183,7 @@
     </row>
     <row r="240" spans="1:5">
       <c r="A240" s="4" t="s">
-        <v>442</v>
+        <v>211</v>
       </c>
       <c r="B240">
         <v>0</v>
@@ -11139,7 +11201,7 @@
     </row>
     <row r="241" spans="1:5">
       <c r="A241" s="4" t="s">
-        <v>443</v>
+        <v>212</v>
       </c>
       <c r="B241">
         <v>0</v>
@@ -11157,7 +11219,7 @@
     </row>
     <row r="242" spans="1:5">
       <c r="A242" s="4" t="s">
-        <v>444</v>
+        <v>437</v>
       </c>
       <c r="B242">
         <v>0</v>
@@ -11175,7 +11237,7 @@
     </row>
     <row r="243" spans="1:5">
       <c r="A243" s="4" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="B243">
         <v>0</v>
@@ -11193,7 +11255,7 @@
     </row>
     <row r="244" spans="1:5">
       <c r="A244" s="4" t="s">
-        <v>446</v>
+        <v>439</v>
       </c>
       <c r="B244">
         <v>0</v>
@@ -11211,7 +11273,7 @@
     </row>
     <row r="245" spans="1:5">
       <c r="A245" s="4" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="B245">
         <v>0</v>
@@ -11229,7 +11291,7 @@
     </row>
     <row r="246" spans="1:5">
       <c r="A246" s="4" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
       <c r="B246">
         <v>0</v>
@@ -11247,7 +11309,7 @@
     </row>
     <row r="247" spans="1:5">
       <c r="A247" s="4" t="s">
-        <v>449</v>
+        <v>442</v>
       </c>
       <c r="B247">
         <v>0</v>
@@ -11265,7 +11327,7 @@
     </row>
     <row r="248" spans="1:5">
       <c r="A248" s="4" t="s">
-        <v>450</v>
+        <v>443</v>
       </c>
       <c r="B248">
         <v>0</v>
@@ -11283,13 +11345,13 @@
     </row>
     <row r="249" spans="1:5">
       <c r="A249" s="4" t="s">
-        <v>451</v>
+        <v>444</v>
       </c>
       <c r="B249">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C249">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D249">
         <v>0</v>
@@ -11301,13 +11363,13 @@
     </row>
     <row r="250" spans="1:5">
       <c r="A250" s="4" t="s">
-        <v>452</v>
+        <v>445</v>
       </c>
       <c r="B250">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C250">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D250">
         <v>0</v>
@@ -11319,13 +11381,13 @@
     </row>
     <row r="251" spans="1:5">
       <c r="A251" s="4" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
       <c r="B251">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C251">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D251">
         <v>0</v>
@@ -11337,13 +11399,13 @@
     </row>
     <row r="252" spans="1:5">
       <c r="A252" s="4" t="s">
-        <v>454</v>
+        <v>447</v>
       </c>
       <c r="B252">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C252">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D252">
         <v>0</v>
@@ -11355,13 +11417,13 @@
     </row>
     <row r="253" spans="1:5">
       <c r="A253" s="4" t="s">
-        <v>455</v>
+        <v>448</v>
       </c>
       <c r="B253">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C253">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D253">
         <v>0</v>
@@ -11373,13 +11435,13 @@
     </row>
     <row r="254" spans="1:5">
       <c r="A254" s="4" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="B254">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C254">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D254">
         <v>0</v>
@@ -11391,13 +11453,13 @@
     </row>
     <row r="255" spans="1:5">
       <c r="A255" s="4" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
       <c r="B255">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C255">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D255">
         <v>0</v>
@@ -11409,7 +11471,7 @@
     </row>
     <row r="256" spans="1:5">
       <c r="A256" s="4" t="s">
-        <v>160</v>
+        <v>451</v>
       </c>
       <c r="B256">
         <v>1</v>
@@ -11427,7 +11489,7 @@
     </row>
     <row r="257" spans="1:5">
       <c r="A257" s="4" t="s">
-        <v>255</v>
+        <v>452</v>
       </c>
       <c r="B257">
         <v>1</v>
@@ -11445,7 +11507,7 @@
     </row>
     <row r="258" spans="1:5">
       <c r="A258" s="4" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="B258">
         <v>1</v>
@@ -11463,7 +11525,7 @@
     </row>
     <row r="259" spans="1:5">
       <c r="A259" s="4" t="s">
-        <v>254</v>
+        <v>454</v>
       </c>
       <c r="B259">
         <v>1</v>
@@ -11481,7 +11543,7 @@
     </row>
     <row r="260" spans="1:5">
       <c r="A260" s="4" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="B260">
         <v>1</v>
@@ -11499,7 +11561,7 @@
     </row>
     <row r="261" spans="1:5">
       <c r="A261" s="4" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="B261">
         <v>1</v>
@@ -11517,7 +11579,7 @@
     </row>
     <row r="262" spans="1:5">
       <c r="A262" s="4" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="B262">
         <v>1</v>
@@ -11535,7 +11597,7 @@
     </row>
     <row r="263" spans="1:5">
       <c r="A263" s="4" t="s">
-        <v>462</v>
+        <v>160</v>
       </c>
       <c r="B263">
         <v>1</v>
@@ -11553,33 +11615,159 @@
     </row>
     <row r="264" spans="1:5">
       <c r="A264" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="B264">
+        <v>1</v>
+      </c>
+      <c r="C264">
+        <v>0</v>
+      </c>
+      <c r="D264">
+        <v>0</v>
+      </c>
+      <c r="E264" s="2" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="265" spans="1:5">
+      <c r="A265" s="4" t="s">
+        <v>458</v>
+      </c>
+      <c r="B265">
+        <v>1</v>
+      </c>
+      <c r="C265">
+        <v>0</v>
+      </c>
+      <c r="D265">
+        <v>0</v>
+      </c>
+      <c r="E265" s="2" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="266" spans="1:5">
+      <c r="A266" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="B266">
+        <v>1</v>
+      </c>
+      <c r="C266">
+        <v>0</v>
+      </c>
+      <c r="D266">
+        <v>0</v>
+      </c>
+      <c r="E266" s="2" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="267" spans="1:5">
+      <c r="A267" s="4" t="s">
+        <v>459</v>
+      </c>
+      <c r="B267">
+        <v>1</v>
+      </c>
+      <c r="C267">
+        <v>0</v>
+      </c>
+      <c r="D267">
+        <v>0</v>
+      </c>
+      <c r="E267" s="2" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="268" spans="1:5">
+      <c r="A268" s="4" t="s">
+        <v>460</v>
+      </c>
+      <c r="B268">
+        <v>1</v>
+      </c>
+      <c r="C268">
+        <v>0</v>
+      </c>
+      <c r="D268">
+        <v>0</v>
+      </c>
+      <c r="E268" s="2" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="269" spans="1:5">
+      <c r="A269" s="4" t="s">
+        <v>461</v>
+      </c>
+      <c r="B269">
+        <v>1</v>
+      </c>
+      <c r="C269">
+        <v>0</v>
+      </c>
+      <c r="D269">
+        <v>0</v>
+      </c>
+      <c r="E269" s="2" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="270" spans="1:5">
+      <c r="A270" s="4" t="s">
+        <v>462</v>
+      </c>
+      <c r="B270">
+        <v>1</v>
+      </c>
+      <c r="C270">
+        <v>0</v>
+      </c>
+      <c r="D270">
+        <v>0</v>
+      </c>
+      <c r="E270" s="2" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="271" spans="1:5">
+      <c r="A271" s="4" t="s">
         <v>463</v>
       </c>
-      <c r="B264">
-        <v>1</v>
-      </c>
-      <c r="C264">
-        <v>0</v>
-      </c>
-      <c r="D264">
-        <v>0</v>
-      </c>
-      <c r="E264" s="2" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="265" spans="1:5">
-      <c r="A265" s="5"/>
-    </row>
-    <row r="266" spans="1:5">
-      <c r="A266" s="5"/>
-    </row>
-    <row r="267" spans="1:5">
-      <c r="A267" s="5"/>
-    </row>
-    <row r="268" spans="1:5">
-      <c r="A268" s="5"/>
+      <c r="B271">
+        <v>1</v>
+      </c>
+      <c r="C271">
+        <v>0</v>
+      </c>
+      <c r="D271">
+        <v>0</v>
+      </c>
+      <c r="E271" s="2" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="272" spans="1:5">
+      <c r="A272" s="5"/>
+    </row>
+    <row r="273" spans="1:1">
+      <c r="A273" s="5"/>
+    </row>
+    <row r="274" spans="1:1">
+      <c r="A274" s="5"/>
+    </row>
+    <row r="275" spans="1:1">
+      <c r="A275" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>